<commit_message>
Login TC - Get Expected Text from Excel
</commit_message>
<xml_diff>
--- a/PayRollProjectDemo/src/main/resources/Excel/TestData.xlsx
+++ b/PayRollProjectDemo/src/main/resources/Excel/TestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="User Details" sheetId="1" r:id="rId1"/>
     <sheet name="Client Details" sheetId="2" r:id="rId2"/>
     <sheet name="Worker Details" sheetId="3" r:id="rId3"/>
     <sheet name="TimeSheet Details" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>UserName</t>
   </si>
@@ -167,6 +168,18 @@
   </si>
   <si>
     <t>bill</t>
+  </si>
+  <si>
+    <t>Welcome to Payroll Application</t>
+  </si>
+  <si>
+    <t>Incorrect username or password.</t>
+  </si>
+  <si>
+    <t>validLogin</t>
+  </si>
+  <si>
+    <t>invalidLogin</t>
   </si>
 </sst>
 </file>
@@ -534,15 +547,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -559,6 +572,22 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -850,4 +879,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Read Expected data from Excel
</commit_message>
<xml_diff>
--- a/PayRollProjectDemo/src/main/resources/Excel/TestData.xlsx
+++ b/PayRollProjectDemo/src/main/resources/Excel/TestData.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Details" sheetId="1" r:id="rId1"/>
     <sheet name="Client Details" sheetId="2" r:id="rId2"/>
     <sheet name="Worker Details" sheetId="3" r:id="rId3"/>
     <sheet name="TimeSheet Details" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Dashboard Details" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>UserName</t>
   </si>
@@ -180,6 +180,42 @@
   </si>
   <si>
     <t>invalidLogin</t>
+  </si>
+  <si>
+    <t>SuccessfulLogout</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>timeSheetPageTitle</t>
+  </si>
+  <si>
+    <t>TIMESHEETS</t>
+  </si>
+  <si>
+    <t>Are you sure you want to generate payslip?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PayslipAlert </t>
+  </si>
+  <si>
+    <t>invoiceAlert</t>
+  </si>
+  <si>
+    <t>Payslip generated!!!</t>
+  </si>
+  <si>
+    <t>PaySlipGenerateSuccess</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete this item?</t>
+  </si>
+  <si>
+    <t>DeleteAlertMessage</t>
+  </si>
+  <si>
+    <t>Are you sure you want to generate invoice?</t>
   </si>
 </sst>
 </file>
@@ -549,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +804,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -775,16 +819,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -874,6 +918,38 @@
       </c>
       <c r="B11" s="2">
         <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -883,12 +959,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>